<commit_message>
added previous balance in customer retention and made changes in the balance drop formula
</commit_message>
<xml_diff>
--- a/uploads/sample/Customer-Retention_v1.4.xlsx
+++ b/uploads/sample/Customer-Retention_v1.4.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Customer Name</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Contact no</t>
+  </si>
+  <si>
+    <t>Previous balance</t>
   </si>
   <si>
     <t>Current balance</t>
@@ -102,7 +105,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -130,6 +133,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,12 +182,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,10 +212,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -283,10 +295,13 @@
       <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1234</v>
@@ -295,22 +310,22 @@
         <v>96932564</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>7506260369</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
+        <v>200000</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>200000</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>23</v>
@@ -319,31 +334,34 @@
         <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="S2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="T2" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>25</v>
+      <c r="U2" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>